<commit_message>
made some homework. yippee koolay
</commit_message>
<xml_diff>
--- a/algoritmit/kt1.xlsx
+++ b/algoritmit/kt1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="T1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>T1</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>century</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
   <si>
     <t>T6</t>
@@ -624,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,10 +972,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,11 +1152,6 @@
       <c r="F10" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1172,7 +1164,7 @@
   <dimension ref="A2:S2"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,15 +1253,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1280,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1288,7 +1280,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1343,7 +1335,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1351,7 +1343,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1405,7 +1397,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1413,7 +1405,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1467,7 +1459,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1475,7 +1467,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1529,7 +1521,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1537,7 +1529,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1591,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1599,7 +1591,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1653,7 +1645,7 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1661,7 +1653,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1715,7 +1707,7 @@
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1723,7 +1715,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1777,7 +1769,7 @@
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1785,7 +1777,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1839,7 +1831,7 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1847,7 +1839,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39">
         <v>1</v>

</xml_diff>